<commit_message>
Fixed bug to read key correctly. Added Java sequential implementation
</commit_message>
<xml_diff>
--- a/speedup_record.xlsx
+++ b/speedup_record.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>TEST</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Java threads</t>
   </si>
   <si>
+    <t>Java ForkJoin</t>
+  </si>
+  <si>
     <t>Cipher</t>
   </si>
   <si>
@@ -51,9 +54,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
@@ -80,6 +83,51 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -88,23 +136,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -118,9 +173,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -135,52 +197,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -193,21 +211,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -224,25 +227,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -254,55 +383,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -314,91 +401,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,17 +412,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -434,15 +426,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -471,17 +454,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -501,11 +478,37 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -514,139 +517,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -988,10 +991,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79816513761468" defaultRowHeight="12.5" outlineLevelRow="3"/>
@@ -1001,7 +1004,7 @@
     <col min="5" max="5" width="10.605504587156"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1025,25 +1028,29 @@
         <v>5</v>
       </c>
       <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>2500.9</v>
@@ -1056,23 +1063,30 @@
       </c>
       <c r="E3">
         <v>1004.1843</v>
+      </c>
+      <c r="H3">
+        <v>504.6</v>
+      </c>
+      <c r="I3">
+        <v>704</v>
       </c>
     </row>
     <row r="4" spans="4:5">
       <c r="D4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added Java threads implementation
</commit_message>
<xml_diff>
--- a/speedup_record.xlsx
+++ b/speedup_record.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>TEST</t>
   </si>
@@ -54,10 +54,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -77,6 +77,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -84,6 +91,53 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -91,23 +145,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -122,93 +169,46 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -221,187 +221,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,6 +412,60 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -433,23 +487,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -457,38 +496,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -503,24 +512,21 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -529,130 +535,124 @@
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -994,7 +994,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79816513761468" defaultRowHeight="12.5" outlineLevelRow="3"/>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:11">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
         <v>7</v>
@@ -1047,8 +1047,26 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1069,6 +1087,12 @@
       </c>
       <c r="I3">
         <v>704</v>
+      </c>
+      <c r="J3">
+        <v>210.6</v>
+      </c>
+      <c r="K3">
+        <v>212.6</v>
       </c>
     </row>
     <row r="4" spans="4:5">

</xml_diff>

<commit_message>
Add Java ForkJoin implementation
</commit_message>
<xml_diff>
--- a/speedup_record.xlsx
+++ b/speedup_record.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>TEST</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Decipher</t>
   </si>
   <si>
+    <t>CIpher</t>
+  </si>
+  <si>
     <t>book.pdf</t>
   </si>
   <si>
@@ -54,10 +57,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -71,13 +74,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -98,17 +94,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -122,6 +123,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -132,29 +155,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -168,8 +168,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -182,31 +199,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,25 +224,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -251,19 +374,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -275,133 +398,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,6 +415,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -430,30 +442,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -465,6 +453,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -493,22 +501,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,142 +520,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -994,7 +997,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79816513761468" defaultRowHeight="12.5" outlineLevelRow="3"/>
@@ -1033,7 +1036,7 @@
       </c>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:13">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
         <v>7</v>
@@ -1065,10 +1068,16 @@
       <c r="K2" t="s">
         <v>8</v>
       </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>2500.9</v>
@@ -1082,6 +1091,12 @@
       <c r="E3">
         <v>1004.1843</v>
       </c>
+      <c r="F3">
+        <v>0.0089</v>
+      </c>
+      <c r="G3">
+        <v>0.0099</v>
+      </c>
       <c r="H3">
         <v>504.6</v>
       </c>
@@ -1093,14 +1108,20 @@
       </c>
       <c r="K3">
         <v>212.6</v>
+      </c>
+      <c r="L3">
+        <v>203.8</v>
+      </c>
+      <c r="M3">
+        <v>219.3</v>
       </c>
     </row>
     <row r="4" spans="4:5">
       <c r="D4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>